<commit_message>
Code changes for testing Sikuli on Win 10
</commit_message>
<xml_diff>
--- a/TestData/AmortTemplateUniversal HD.xlsx
+++ b/TestData/AmortTemplateUniversal HD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\amort test\AmortTemplateAutomation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\206534643\git\AmortTemplateAutomation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="41">
   <si>
     <t>AmortTemplateName</t>
   </si>
@@ -148,25 +148,10 @@
     <t>Acquired Originals (old)</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>T</t>
-  </si>
-  <si>
-    <t>Original Series (Season 2-3)</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
 </sst>
 </file>
@@ -493,11 +478,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -560,19 +543,19 @@
         <v>15</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F2" s="3">
         <v>12</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="3">
         <v>0</v>
@@ -584,162 +567,10 @@
         <v>11</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>128</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="3">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="H3" s="3">
-        <v>12</v>
-      </c>
-      <c r="I3" s="3">
-        <v>0</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>132</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="3">
-        <v>12</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H4" s="3">
-        <v>60</v>
-      </c>
-      <c r="I4" s="3">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
-        <v>133</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="3">
-        <v>12</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
-        <v>122</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3">
-        <v>12</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H6" s="3">
-        <v>60</v>
-      </c>
-      <c r="I6" s="3">
-        <v>0</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>